<commit_message>
adding in array questions and some changes 9feb
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\Desktop\dsa cheetshhet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA2241E-54A5-44A6-A4A8-CC708028ED6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -1857,18 +1860,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1891,7 +1894,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21">
@@ -1902,7 +1905,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -1913,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -1924,7 +1927,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1935,7 +1938,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -1946,7 +1949,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -1957,7 +1960,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -1968,7 +1971,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -1979,7 +1982,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -1990,7 +1993,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
@@ -2001,7 +2004,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21">
@@ -2012,7 +2015,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2023,7 +2026,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2034,7 +2037,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2045,7 +2048,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -2056,7 +2059,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
@@ -2067,7 +2070,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2078,7 +2081,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2089,7 +2092,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
@@ -2100,7 +2103,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
@@ -2111,7 +2114,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21">
@@ -2122,7 +2125,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21">

</xml_diff>

<commit_message>
optimizing and new programs 10feb
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayush\Desktop\dsa cheetshhet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA2241E-54A5-44A6-A4A8-CC708028ED6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D2FDE3-6F13-48A5-A799-EEB31E6633D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="471">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1429,6 +1429,21 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>not done</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> done</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>need to be optimized</t>
   </si>
 </sst>
 </file>
@@ -1860,8 +1875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2070,7 +2085,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2081,7 +2096,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2136,7 +2151,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>4</v>
+        <v>466</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21">
@@ -2147,7 +2162,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">
@@ -2158,7 +2173,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21">
@@ -2169,7 +2184,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2180,7 +2195,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">
@@ -2191,7 +2206,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21">
@@ -2202,7 +2217,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21">
@@ -2213,7 +2228,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>4</v>
+        <v>468</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
@@ -2224,7 +2239,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>4</v>
+        <v>469</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21">
@@ -2235,7 +2250,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>4</v>
+        <v>468</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
@@ -2246,7 +2261,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">
@@ -2257,7 +2272,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>4</v>
+        <v>468</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
@@ -2268,7 +2283,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>4</v>
+        <v>468</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -2279,7 +2294,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>4</v>
+        <v>468</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
@@ -2290,21 +2305,17 @@
         <v>41</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">
       <c r="B42" s="7"/>
-      <c r="C42" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" ht="21">
       <c r="A43" s="5"/>
       <c r="B43" s="7"/>
-      <c r="C43" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" ht="21">
       <c r="A44" s="8" t="s">

</xml_diff>